<commit_message>
Finished REQ12523 and REQ12525.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.80.30.20_UserOptionsWithDifferentLanguageOption.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.80.30.20_UserOptionsWithDifferentLanguageOption.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="2535" windowWidth="18195" windowHeight="14070"/>
+    <workbookView xWindow="-1635" yWindow="0" windowWidth="18195" windowHeight="14070"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="3" r:id="rId1"/>
@@ -3602,6 +3602,17 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>NformLogin</t>
+  </si>
+  <si>
+    <t>Running Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sashimi</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>;Fill up the field information required to add a new user.</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -3614,9 +3625,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NformLogin</t>
-  </si>
-  <si>
     <t>"Administrator"</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -3637,66 +3645,58 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>;Set language by user option.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Text</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>Equal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>English -- English</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>German -- Deutsch</t>
+  </si>
+  <si>
+    <t>Close</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Application</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Equal</t>
+    <t>;Verify the settings.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T</t>
+    <t>;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Running Range</t>
+    <t>Anwendung</t>
+  </si>
+  <si>
+    <t>;Reset language by user option.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sashimi</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <t>Application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>;Clear</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Set language by user option.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>English -- English</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Verify the settings.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;Reset language by user option.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Application</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>German -- Deutsch</t>
-  </si>
-  <si>
-    <t>Anwendung</t>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Close</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3911,7 +3911,35 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4709,7 +4737,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -4728,29 +4756,29 @@
         <v>754</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>805</v>
+        <v>793</v>
       </c>
       <c r="C3" s="4">
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -4769,10 +4797,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="F4" s="14">
         <v>5</v>
@@ -4798,7 +4826,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -4876,7 +4904,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="2" t="s">
-        <v>804</v>
+        <v>792</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="4">
@@ -4895,13 +4923,13 @@
         <v>7</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -4918,10 +4946,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="F9" s="14">
         <v>5</v>
@@ -4958,7 +4986,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="4"/>
@@ -4987,7 +5015,7 @@
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>815</v>
+        <v>808</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -5067,7 +5095,7 @@
         <v>19</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>801</v>
+        <v>809</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>2</v>
@@ -5119,23 +5147,23 @@
         <v>15</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -5152,7 +5180,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -5235,7 +5263,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>714</v>
@@ -5276,13 +5304,13 @@
         <v>7</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
@@ -5305,7 +5333,7 @@
         <v>714</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>815</v>
+        <v>808</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>2</v>
@@ -5324,7 +5352,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="4"/>
@@ -5405,13 +5433,13 @@
         <v>7</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -5436,7 +5464,7 @@
         <v>13</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="I27" s="14"/>
       <c r="J27" s="4"/>
@@ -5531,7 +5559,7 @@
         <v>19</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>801</v>
+        <v>809</v>
       </c>
       <c r="G31" s="14" t="s">
         <v>2</v>
@@ -5573,23 +5601,23 @@
         <v>32</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -5601,7 +5629,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
@@ -5679,13 +5707,13 @@
         <v>7</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -5703,7 +5731,7 @@
         <v>714</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>815</v>
+        <v>808</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>2</v>
@@ -5721,7 +5749,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>806</v>
+        <v>815</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="14"/>
@@ -5739,10 +5767,10 @@
         <v>39</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="F40" s="14">
         <v>5</v>
@@ -5758,11 +5786,19 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="N2:N8 N11 N14:N40">
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N2:N9 N12:N35">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N8 N11 N14:N40">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>